<commit_message>
Cleaning up files and folders.
</commit_message>
<xml_diff>
--- a/Calibration/Testing/Testing_Moore_et_al_1998.xlsx
+++ b/Calibration/Testing/Testing_Moore_et_al_1998.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - University of Cambridge\!!!!!!PHD\Fissure8_MI_Work\MagmaSat\Testing_Compiled_FinalOnes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Manuscripts in Progress/__VESIcal/__TheCode/VESIcal/Calibration/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF1F594-8C35-424C-8409-0F4C946BBCD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE07D14B-39C8-2A4B-9AA1-13BE80609696}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{E4D1C9D5-0A60-45B0-90AE-883D25AC4827}"/>
+    <workbookView xWindow="2640" yWindow="1080" windowWidth="22980" windowHeight="23700" xr2:uid="{E4D1C9D5-0A60-45B0-90AE-883D25AC4827}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -349,7 +349,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,12 +382,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -857,17 +851,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="21" max="21" width="29.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="21" max="21" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
@@ -932,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -997,7 +991,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1062,7 +1056,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1127,7 +1121,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -1192,7 +1186,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1257,7 +1251,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1322,7 +1316,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1387,7 +1381,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -1452,7 +1446,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1517,7 +1511,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1582,7 +1576,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -1647,7 +1641,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1712,7 +1706,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1777,7 +1771,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1842,7 +1836,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
@@ -1907,7 +1901,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1972,7 +1966,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -2037,7 +2031,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>41</v>
       </c>
@@ -2102,7 +2096,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
@@ -2167,7 +2161,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2232,7 +2226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2297,7 +2291,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -2354,7 +2348,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2411,7 +2405,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -2468,7 +2462,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -2533,7 +2527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -2598,7 +2592,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
@@ -2663,7 +2657,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
@@ -2728,7 +2722,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2738,8 +2732,9 @@
       <c r="D30">
         <v>12.5</v>
       </c>
-      <c r="F30" s="9">
-        <v>1</v>
+      <c r="F30" s="9"/>
+      <c r="G30">
+        <v>5.2</v>
       </c>
       <c r="J30">
         <v>0.5</v>
@@ -2775,7 +2770,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -2822,7 +2817,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -2869,7 +2864,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -2916,7 +2911,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2963,7 +2958,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -3024,7 +3019,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -3085,7 +3080,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>66</v>
       </c>
@@ -3148,7 +3143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>68</v>
       </c>
@@ -3211,7 +3206,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -3276,7 +3271,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -3341,7 +3336,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -3406,7 +3401,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -3481,20 +3476,20 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="98" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="15" width="8.88671875" style="15"/>
-    <col min="16" max="16" width="8.88671875" style="29"/>
-    <col min="17" max="18" width="8.88671875" style="30"/>
-    <col min="19" max="16384" width="8.88671875" style="15"/>
+    <col min="1" max="15" width="8.83203125" style="15"/>
+    <col min="16" max="16" width="8.83203125" style="29"/>
+    <col min="17" max="18" width="8.83203125" style="30"/>
+    <col min="19" max="16384" width="8.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>79</v>
       </c>
@@ -3553,7 +3548,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -3613,7 +3608,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -3673,7 +3668,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -3733,7 +3728,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -3793,7 +3788,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -3853,7 +3848,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -3913,7 +3908,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -3973,7 +3968,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -4021,7 +4016,7 @@
         <v>98.289999999999992</v>
       </c>
       <c r="P9" s="31">
-        <v>496.32424926757813</v>
+        <v>496.32424926757812</v>
       </c>
       <c r="Q9" s="18">
         <v>7.3575608432292938E-2</v>
@@ -4033,7 +4028,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -4093,7 +4088,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -4153,7 +4148,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -4213,7 +4208,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -4273,7 +4268,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -4333,7 +4328,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -4393,7 +4388,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -4453,7 +4448,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -4513,7 +4508,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -4573,7 +4568,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -4633,7 +4628,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -4693,7 +4688,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -4753,7 +4748,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -4813,7 +4808,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -4873,7 +4868,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -4933,7 +4928,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -4993,7 +4988,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -5053,7 +5048,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -5113,7 +5108,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:24" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -5173,7 +5168,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -5236,7 +5231,7 @@
       <c r="W29" s="18"/>
       <c r="X29" s="17"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -5299,7 +5294,7 @@
       <c r="W30" s="18"/>
       <c r="X30" s="17"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -5362,7 +5357,7 @@
       <c r="W31" s="18"/>
       <c r="X31" s="17"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -5425,7 +5420,7 @@
       <c r="W32" s="18"/>
       <c r="X32" s="17"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -5488,7 +5483,7 @@
       <c r="W33" s="18"/>
       <c r="X33" s="17"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -5551,7 +5546,7 @@
       <c r="W34" s="18"/>
       <c r="X34" s="17"/>
     </row>
-    <row r="35" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -5614,7 +5609,7 @@
       <c r="W35" s="18"/>
       <c r="X35" s="17"/>
     </row>
-    <row r="36" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -5674,7 +5669,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -5722,7 +5717,7 @@
         <v>98.289999999999992</v>
       </c>
       <c r="P37" s="31">
-        <v>287.05374145507813</v>
+        <v>287.05374145507812</v>
       </c>
       <c r="Q37" s="21">
         <v>6.0998063534498215E-2</v>
@@ -5734,7 +5729,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -5782,7 +5777,7 @@
         <v>98.289999999999992</v>
       </c>
       <c r="P38" s="31">
-        <v>333.01504516601563</v>
+        <v>333.01504516601562</v>
       </c>
       <c r="Q38" s="21">
         <v>6.6395796835422516E-2</v>
@@ -5794,7 +5789,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -5848,13 +5843,13 @@
         <v>7.1425721049308777E-2</v>
       </c>
       <c r="R39" s="20">
-        <v>2.0927810668945313</v>
+        <v>2.0927810668945312</v>
       </c>
       <c r="S39" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -5914,7 +5909,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -5974,7 +5969,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -6034,7 +6029,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -6094,7 +6089,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -6154,7 +6149,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -6214,7 +6209,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -6274,7 +6269,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -6334,7 +6329,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="15">
         <v>47</v>
       </c>
@@ -6394,7 +6389,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="15">
         <v>48</v>
       </c>
@@ -6454,7 +6449,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="15">
         <v>49</v>
       </c>
@@ -6514,7 +6509,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" s="15">
         <v>50</v>
       </c>
@@ -6574,7 +6569,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" s="15">
         <v>51</v>
       </c>
@@ -6634,7 +6629,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="15">
         <v>52</v>
       </c>
@@ -6694,7 +6689,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="15">
         <v>53</v>
       </c>
@@ -6754,7 +6749,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="15">
         <v>54</v>
       </c>
@@ -6814,7 +6809,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="15">
         <v>55</v>
       </c>
@@ -6879,7 +6874,7 @@
       <c r="X56" s="21"/>
       <c r="Y56" s="20"/>
     </row>
-    <row r="57" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="15">
         <v>56</v>
       </c>
@@ -6944,7 +6939,7 @@
       <c r="X57" s="21"/>
       <c r="Y57" s="20"/>
     </row>
-    <row r="58" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="15">
         <v>57</v>
       </c>
@@ -7009,7 +7004,7 @@
       <c r="X58" s="26"/>
       <c r="Y58" s="25"/>
     </row>
-    <row r="59" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="15">
         <v>58</v>
       </c>
@@ -7074,7 +7069,7 @@
       <c r="X59" s="26"/>
       <c r="Y59" s="25"/>
     </row>
-    <row r="60" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="15">
         <v>59</v>
       </c>
@@ -7141,7 +7136,7 @@
       <c r="X60" s="21"/>
       <c r="Y60" s="20"/>
     </row>
-    <row r="61" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="15">
         <v>60</v>
       </c>
@@ -7206,7 +7201,7 @@
       <c r="X61" s="21"/>
       <c r="Y61" s="20"/>
     </row>
-    <row r="62" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="15">
         <v>61</v>
       </c>
@@ -7271,7 +7266,7 @@
       <c r="X62" s="21"/>
       <c r="Y62" s="20"/>
     </row>
-    <row r="63" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="15">
         <v>62</v>
       </c>
@@ -7336,7 +7331,7 @@
       <c r="X63" s="21"/>
       <c r="Y63" s="20"/>
     </row>
-    <row r="64" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="15">
         <v>63</v>
       </c>
@@ -7401,7 +7396,7 @@
       <c r="X64" s="26"/>
       <c r="Y64" s="25"/>
     </row>
-    <row r="65" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="15">
         <v>64</v>
       </c>
@@ -7461,7 +7456,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="15">
         <v>65</v>
       </c>
@@ -7521,7 +7516,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="15">
         <v>66</v>
       </c>

</xml_diff>